<commit_message>
JLG Loan + stabalization
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/3508-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-None-INSTALLMENT-FEE-FLAT-WaiveCharge-Charges.xlsx
+++ b/Mifos Automation Excels/Client/3508-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-None-INSTALLMENT-FEE-FLAT-WaiveCharge-Charges.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620"/>
+    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Charges" sheetId="9" r:id="rId1"/>
@@ -150,7 +150,6 @@
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -201,9 +200,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -222,16 +218,19 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -557,7 +556,7 @@
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>4000</v>
       </c>
     </row>
@@ -565,7 +564,7 @@
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
     </row>
@@ -573,7 +572,7 @@
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>4000</v>
       </c>
     </row>
@@ -628,80 +627,80 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>10000</v>
       </c>
-      <c r="B2" s="9">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
         <v>10000</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>1581.47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>685.07</v>
       </c>
-      <c r="B3" s="9">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="B3" s="8">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
         <v>685.07</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>193.97</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>1200</v>
       </c>
-      <c r="B4" s="9">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>100</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="B4" s="8">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8">
+        <v>100</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
         <v>1100</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
-        <v>0</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="A5" s="8">
+        <v>0</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
         <v>0</v>
       </c>
     </row>
@@ -777,24 +776,24 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>42005</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>10000</v>
       </c>
       <c r="H2" s="4"/>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>0</v>
       </c>
       <c r="J2" s="4"/>
-      <c r="K2" s="9">
-        <v>0</v>
-      </c>
-      <c r="L2" s="9">
+      <c r="K2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
         <v>0</v>
       </c>
       <c r="M2" s="4"/>
@@ -803,554 +802,554 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>31</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>42036</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>785.8</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>9214.2000000000007</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>101.92</v>
       </c>
-      <c r="I3" s="9">
-        <v>100</v>
-      </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-      <c r="K3" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L3" s="9">
-        <v>0</v>
-      </c>
-      <c r="M3" s="9">
-        <v>0</v>
-      </c>
-      <c r="N3" s="9">
-        <v>0</v>
-      </c>
-      <c r="O3" s="9">
-        <v>100</v>
-      </c>
-      <c r="P3" s="9">
+      <c r="I3" s="8">
+        <v>100</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L3" s="8">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+      <c r="N3" s="8">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8">
+        <v>100</v>
+      </c>
+      <c r="P3" s="8">
         <v>887.72</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>28</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>42064</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>795.67</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>8418.5300000000007</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>92.05</v>
       </c>
-      <c r="I4" s="9">
-        <v>100</v>
-      </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0</v>
-      </c>
-      <c r="N4" s="9">
-        <v>0</v>
-      </c>
-      <c r="O4" s="9">
-        <v>0</v>
-      </c>
-      <c r="P4" s="9">
+      <c r="I4" s="8">
+        <v>100</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0</v>
+      </c>
+      <c r="M4" s="8">
+        <v>0</v>
+      </c>
+      <c r="N4" s="8">
+        <v>0</v>
+      </c>
+      <c r="O4" s="8">
+        <v>0</v>
+      </c>
+      <c r="P4" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>31</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>42095</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>785.8</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>7632.73</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>101.92</v>
       </c>
-      <c r="I5" s="9">
-        <v>100</v>
-      </c>
-      <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="9">
-        <v>0</v>
-      </c>
-      <c r="N5" s="9">
-        <v>0</v>
-      </c>
-      <c r="O5" s="9">
-        <v>0</v>
-      </c>
-      <c r="P5" s="9">
+      <c r="I5" s="8">
+        <v>100</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0</v>
+      </c>
+      <c r="P5" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>30</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>42125</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>812.44</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>6820.29</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>75.28</v>
       </c>
-      <c r="I6" s="9">
-        <v>100</v>
-      </c>
-      <c r="J6" s="9">
-        <v>0</v>
-      </c>
-      <c r="K6" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L6" s="9">
-        <v>0</v>
-      </c>
-      <c r="M6" s="9">
-        <v>0</v>
-      </c>
-      <c r="N6" s="9">
-        <v>0</v>
-      </c>
-      <c r="O6" s="9">
-        <v>0</v>
-      </c>
-      <c r="P6" s="9">
+      <c r="I6" s="8">
+        <v>100</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="N6" s="8">
+        <v>0</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0</v>
+      </c>
+      <c r="P6" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>31</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>42156</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>818.21</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>6002.08</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>69.510000000000005</v>
       </c>
-      <c r="I7" s="9">
-        <v>100</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0</v>
-      </c>
-      <c r="K7" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L7" s="9">
-        <v>0</v>
-      </c>
-      <c r="M7" s="9">
-        <v>0</v>
-      </c>
-      <c r="N7" s="9">
-        <v>0</v>
-      </c>
-      <c r="O7" s="9">
-        <v>0</v>
-      </c>
-      <c r="P7" s="9">
+      <c r="I7" s="8">
+        <v>100</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0</v>
+      </c>
+      <c r="P7" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>30</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>42186</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>828.52</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>5173.5600000000004</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <v>59.2</v>
       </c>
-      <c r="I8" s="9">
-        <v>100</v>
-      </c>
-      <c r="J8" s="9">
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L8" s="9">
-        <v>0</v>
-      </c>
-      <c r="M8" s="9">
-        <v>0</v>
-      </c>
-      <c r="N8" s="9">
-        <v>0</v>
-      </c>
-      <c r="O8" s="9">
-        <v>0</v>
-      </c>
-      <c r="P8" s="9">
+      <c r="I8" s="8">
+        <v>100</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>31</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>42217</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>834.99</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>4338.57</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>52.73</v>
       </c>
-      <c r="I9" s="9">
-        <v>100</v>
-      </c>
-      <c r="J9" s="9">
-        <v>0</v>
-      </c>
-      <c r="K9" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L9" s="9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="9">
-        <v>0</v>
-      </c>
-      <c r="N9" s="9">
-        <v>0</v>
-      </c>
-      <c r="O9" s="9">
-        <v>0</v>
-      </c>
-      <c r="P9" s="9">
+      <c r="I9" s="8">
+        <v>100</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>0</v>
+      </c>
+      <c r="N9" s="8">
+        <v>0</v>
+      </c>
+      <c r="O9" s="8">
+        <v>0</v>
+      </c>
+      <c r="P9" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>31</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>42248</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>843.5</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>3495.07</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>44.22</v>
       </c>
-      <c r="I10" s="9">
-        <v>100</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0</v>
-      </c>
-      <c r="K10" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L10" s="9">
-        <v>0</v>
-      </c>
-      <c r="M10" s="9">
-        <v>0</v>
-      </c>
-      <c r="N10" s="9">
-        <v>0</v>
-      </c>
-      <c r="O10" s="9">
-        <v>0</v>
-      </c>
-      <c r="P10" s="9">
+      <c r="I10" s="8">
+        <v>100</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L10" s="8">
+        <v>0</v>
+      </c>
+      <c r="M10" s="8">
+        <v>0</v>
+      </c>
+      <c r="N10" s="8">
+        <v>0</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0</v>
+      </c>
+      <c r="P10" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>30</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>42278</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>853.25</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>2641.82</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>34.47</v>
       </c>
-      <c r="I11" s="9">
-        <v>100</v>
-      </c>
-      <c r="J11" s="9">
-        <v>0</v>
-      </c>
-      <c r="K11" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L11" s="9">
-        <v>0</v>
-      </c>
-      <c r="M11" s="9">
-        <v>0</v>
-      </c>
-      <c r="N11" s="9">
-        <v>0</v>
-      </c>
-      <c r="O11" s="9">
-        <v>0</v>
-      </c>
-      <c r="P11" s="9">
+      <c r="I11" s="8">
+        <v>100</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0</v>
+      </c>
+      <c r="P11" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>31</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>42309</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>860.8</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <v>1781.02</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>26.92</v>
       </c>
-      <c r="I12" s="9">
-        <v>100</v>
-      </c>
-      <c r="J12" s="9">
-        <v>0</v>
-      </c>
-      <c r="K12" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L12" s="9">
-        <v>0</v>
-      </c>
-      <c r="M12" s="9">
-        <v>0</v>
-      </c>
-      <c r="N12" s="9">
-        <v>0</v>
-      </c>
-      <c r="O12" s="9">
-        <v>0</v>
-      </c>
-      <c r="P12" s="9">
+      <c r="I12" s="8">
+        <v>100</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>0</v>
+      </c>
+      <c r="N12" s="8">
+        <v>0</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0</v>
+      </c>
+      <c r="P12" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>30</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>42339</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>870.15</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>910.87</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>17.57</v>
       </c>
-      <c r="I13" s="9">
-        <v>100</v>
-      </c>
-      <c r="J13" s="9">
-        <v>0</v>
-      </c>
-      <c r="K13" s="9">
-        <v>987.72</v>
-      </c>
-      <c r="L13" s="9">
-        <v>0</v>
-      </c>
-      <c r="M13" s="9">
-        <v>0</v>
-      </c>
-      <c r="N13" s="9">
-        <v>0</v>
-      </c>
-      <c r="O13" s="9">
-        <v>0</v>
-      </c>
-      <c r="P13" s="9">
+      <c r="I13" s="8">
+        <v>100</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>987.72</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0</v>
+      </c>
+      <c r="N13" s="8">
+        <v>0</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0</v>
+      </c>
+      <c r="P13" s="8">
         <v>987.72</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>12</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>31</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>42370</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>910.87</v>
       </c>
-      <c r="G14" s="9">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9">
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
         <v>9.2799999999999994</v>
       </c>
-      <c r="I14" s="9">
-        <v>100</v>
-      </c>
-      <c r="J14" s="9">
-        <v>0</v>
-      </c>
-      <c r="K14" s="10">
+      <c r="I14" s="8">
+        <v>100</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0</v>
+      </c>
+      <c r="K14" s="9">
         <v>1020.15</v>
       </c>
-      <c r="L14" s="9">
-        <v>0</v>
-      </c>
-      <c r="M14" s="9">
-        <v>0</v>
-      </c>
-      <c r="N14" s="9">
-        <v>0</v>
-      </c>
-      <c r="O14" s="9">
-        <v>0</v>
-      </c>
-      <c r="P14" s="10">
+      <c r="L14" s="8">
+        <v>0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>0</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0</v>
+      </c>
+      <c r="P14" s="9">
         <v>1020.15</v>
       </c>
     </row>
@@ -1363,111 +1362,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="13">
         <v>3405</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="14">
         <v>42005</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="5">
-        <v>100</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>100</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="13">
+      <c r="E2" s="13">
+        <v>100</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="13">
+        <v>100</v>
+      </c>
+      <c r="I2" s="13">
+        <v>0</v>
+      </c>
+      <c r="J2" s="15">
         <v>10000</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="13">
         <v>3402</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="14">
         <v>42005</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="15">
         <v>10000</v>
       </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="13">
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15">
         <v>10000</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>